<commit_message>
update topic sheet - Ines
</commit_message>
<xml_diff>
--- a/topic_term_sheet.xlsx
+++ b/topic_term_sheet.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27809"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/inesayara/Desktop/Product/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mreading/workspace/apwa/Product-v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB88DD9-20EB-B04D-91AF-B5DB6E9C4117}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="460" windowWidth="27580" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Terms" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="250">
   <si>
     <t>TOPIC</t>
   </si>
@@ -267,9 +268,6 @@
   </si>
   <si>
     <t>outcasts</t>
-  </si>
-  <si>
-    <t>racial, race</t>
   </si>
   <si>
     <t>cellmate</t>
@@ -785,7 +783,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -846,6 +844,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1048,14 +1049,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:D271"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
-      <selection activeCell="C280" sqref="C280"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1718,7 +1719,7 @@
     </row>
     <row r="83" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B83" s="1" t="s">
-        <v>80</v>
+        <v>180</v>
       </c>
       <c r="C83" s="1">
         <v>3</v>
@@ -1726,7 +1727,7 @@
     </row>
     <row r="84" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B84" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C84" s="1">
         <v>4</v>
@@ -1734,7 +1735,7 @@
     </row>
     <row r="85" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B85" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C85" s="1">
         <v>7</v>
@@ -1742,7 +1743,7 @@
     </row>
     <row r="86" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B86" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C86" s="1">
         <v>10</v>
@@ -1750,7 +1751,7 @@
     </row>
     <row r="87" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B87" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C87" s="1">
         <v>6</v>
@@ -1758,7 +1759,7 @@
     </row>
     <row r="88" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B88" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C88" s="1">
         <v>3</v>
@@ -1766,7 +1767,7 @@
     </row>
     <row r="89" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B89" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C89" s="1">
         <v>7</v>
@@ -1774,7 +1775,7 @@
     </row>
     <row r="90" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B90" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C90" s="1">
         <v>7</v>
@@ -1782,7 +1783,7 @@
     </row>
     <row r="91" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B91" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C91" s="1">
         <v>8</v>
@@ -1790,7 +1791,7 @@
     </row>
     <row r="92" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B92" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C92" s="1">
         <v>9</v>
@@ -1798,7 +1799,7 @@
     </row>
     <row r="93" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B93" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C93" s="1">
         <v>9</v>
@@ -1806,7 +1807,7 @@
     </row>
     <row r="94" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B94" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C94" s="1">
         <v>10</v>
@@ -1814,7 +1815,7 @@
     </row>
     <row r="95" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B95" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C95" s="1">
         <v>8</v>
@@ -1822,7 +1823,7 @@
     </row>
     <row r="96" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B96" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C96" s="1">
         <v>10</v>
@@ -1830,7 +1831,7 @@
     </row>
     <row r="97" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B97" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C97" s="1">
         <v>10.5</v>
@@ -1838,7 +1839,7 @@
     </row>
     <row r="98" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B98" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C98" s="1">
         <v>10.5</v>
@@ -1846,7 +1847,7 @@
     </row>
     <row r="99" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B99" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C99" s="1">
         <v>10.5</v>
@@ -1854,7 +1855,7 @@
     </row>
     <row r="100" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B100" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C100" s="1">
         <v>10.5</v>
@@ -1862,7 +1863,7 @@
     </row>
     <row r="101" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B101" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C101" s="1">
         <v>10.5</v>
@@ -1870,7 +1871,7 @@
     </row>
     <row r="102" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B102" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C102" s="1">
         <v>10.5</v>
@@ -1878,7 +1879,7 @@
     </row>
     <row r="103" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B103" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C103" s="1">
         <v>8</v>
@@ -1886,7 +1887,7 @@
     </row>
     <row r="104" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B104" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C104" s="1">
         <v>10</v>
@@ -1894,7 +1895,7 @@
     </row>
     <row r="105" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B105" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C105" s="1">
         <v>10.5</v>
@@ -1902,7 +1903,7 @@
     </row>
     <row r="106" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B106" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C106" s="1">
         <v>10.5</v>
@@ -1910,7 +1911,7 @@
     </row>
     <row r="107" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B107" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C107" s="1">
         <v>10.5</v>
@@ -1918,7 +1919,7 @@
     </row>
     <row r="108" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B108" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C108" s="1">
         <v>10</v>
@@ -1926,7 +1927,7 @@
     </row>
     <row r="110" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A110" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>6</v>
@@ -1945,7 +1946,7 @@
     </row>
     <row r="112" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B112" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C112" s="1">
         <v>5</v>
@@ -1953,7 +1954,7 @@
     </row>
     <row r="113" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B113" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C113" s="1">
         <v>2</v>
@@ -1961,7 +1962,7 @@
     </row>
     <row r="114" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B114" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C114" s="1">
         <v>3</v>
@@ -1969,7 +1970,7 @@
     </row>
     <row r="115" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B115" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C115" s="1">
         <v>8</v>
@@ -1977,7 +1978,7 @@
     </row>
     <row r="116" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B116" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C116" s="1">
         <v>10.5</v>
@@ -1985,7 +1986,7 @@
     </row>
     <row r="117" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B117" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C117" s="1">
         <v>10.5</v>
@@ -1993,7 +1994,7 @@
     </row>
     <row r="118" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B118" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C118" s="1">
         <v>10</v>
@@ -2001,7 +2002,7 @@
     </row>
     <row r="119" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B119" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C119" s="1">
         <v>4</v>
@@ -2025,7 +2026,7 @@
     </row>
     <row r="122" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B122" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C122" s="1">
         <v>8</v>
@@ -2033,7 +2034,7 @@
     </row>
     <row r="123" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B123" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C123" s="1">
         <v>10.5</v>
@@ -2041,7 +2042,7 @@
     </row>
     <row r="124" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B124" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C124" s="1">
         <v>7</v>
@@ -2057,7 +2058,7 @@
     </row>
     <row r="126" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B126" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C126" s="1">
         <v>4</v>
@@ -2065,7 +2066,7 @@
     </row>
     <row r="127" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B127" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C127" s="1">
         <v>10.5</v>
@@ -2073,7 +2074,7 @@
     </row>
     <row r="128" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B128" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C128" s="1">
         <v>10</v>
@@ -2081,7 +2082,7 @@
     </row>
     <row r="129" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B129" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C129" s="1">
         <v>3</v>
@@ -2089,7 +2090,7 @@
     </row>
     <row r="130" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B130" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C130" s="1">
         <v>7</v>
@@ -2100,10 +2101,10 @@
     </row>
     <row r="132" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A132" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B132" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="B132" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="C132" s="1">
         <v>10.5</v>
@@ -2111,7 +2112,7 @@
     </row>
     <row r="133" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B133" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C133" s="1">
         <v>3</v>
@@ -2119,7 +2120,7 @@
     </row>
     <row r="134" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B134" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C134" s="1">
         <v>1</v>
@@ -2127,7 +2128,7 @@
     </row>
     <row r="135" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B135" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C135" s="1">
         <v>1</v>
@@ -2135,7 +2136,7 @@
     </row>
     <row r="136" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B136" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C136" s="1">
         <v>3</v>
@@ -2143,7 +2144,7 @@
     </row>
     <row r="137" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B137" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C137" s="1">
         <v>11</v>
@@ -2151,7 +2152,7 @@
     </row>
     <row r="138" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B138" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C138" s="1">
         <v>4</v>
@@ -2159,7 +2160,7 @@
     </row>
     <row r="139" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B139" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C139" s="1">
         <v>4</v>
@@ -2167,7 +2168,7 @@
     </row>
     <row r="140" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B140" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C140" s="1">
         <v>10</v>
@@ -2175,7 +2176,7 @@
     </row>
     <row r="141" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B141" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C141" s="1">
         <v>7</v>
@@ -2183,7 +2184,7 @@
     </row>
     <row r="142" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B142" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C142" s="1">
         <v>5</v>
@@ -2191,7 +2192,7 @@
     </row>
     <row r="143" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B143" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C143" s="1">
         <v>5</v>
@@ -2199,7 +2200,7 @@
     </row>
     <row r="144" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B144" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C144" s="1">
         <v>9</v>
@@ -2207,7 +2208,7 @@
     </row>
     <row r="145" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B145" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C145" s="1">
         <v>9</v>
@@ -2215,7 +2216,7 @@
     </row>
     <row r="146" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B146" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C146" s="1">
         <v>8</v>
@@ -2223,7 +2224,7 @@
     </row>
     <row r="147" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B147" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C147" s="1">
         <v>7</v>
@@ -2231,7 +2232,7 @@
     </row>
     <row r="148" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B148" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C148" s="1">
         <v>6</v>
@@ -2239,7 +2240,7 @@
     </row>
     <row r="149" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B149" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C149" s="1">
         <v>5</v>
@@ -2247,7 +2248,7 @@
     </row>
     <row r="150" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B150" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C150" s="1">
         <v>8</v>
@@ -2255,7 +2256,7 @@
     </row>
     <row r="151" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B151" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C151" s="1">
         <v>4</v>
@@ -2263,7 +2264,7 @@
     </row>
     <row r="152" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B152" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C152" s="1">
         <v>7</v>
@@ -2271,7 +2272,7 @@
     </row>
     <row r="153" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B153" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C153" s="1">
         <v>3</v>
@@ -2279,7 +2280,7 @@
     </row>
     <row r="154" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B154" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C154" s="1">
         <v>3</v>
@@ -2287,7 +2288,7 @@
     </row>
     <row r="155" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B155" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C155" s="1">
         <v>10</v>
@@ -2295,7 +2296,7 @@
     </row>
     <row r="156" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B156" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C156" s="1">
         <v>2</v>
@@ -2303,7 +2304,7 @@
     </row>
     <row r="157" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B157" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C157" s="1">
         <v>2</v>
@@ -2311,7 +2312,7 @@
     </row>
     <row r="158" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B158" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C158" s="1">
         <v>5</v>
@@ -2319,7 +2320,7 @@
     </row>
     <row r="159" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B159" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C159" s="1">
         <v>10.5</v>
@@ -2327,7 +2328,7 @@
     </row>
     <row r="160" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B160" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C160" s="1">
         <v>4</v>
@@ -2335,10 +2336,10 @@
     </row>
     <row r="162" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A162" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B162" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="B162" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="C162" s="1">
         <v>1</v>
@@ -2346,7 +2347,7 @@
     </row>
     <row r="163" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B163" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C163" s="1">
         <v>2</v>
@@ -2354,7 +2355,7 @@
     </row>
     <row r="164" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B164" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C164" s="1">
         <v>2</v>
@@ -2362,7 +2363,7 @@
     </row>
     <row r="165" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B165" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C165" s="1">
         <v>3</v>
@@ -2370,7 +2371,7 @@
     </row>
     <row r="166" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B166" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C166" s="1">
         <v>3</v>
@@ -2378,7 +2379,7 @@
     </row>
     <row r="167" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B167" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C167" s="1">
         <v>4</v>
@@ -2386,7 +2387,7 @@
     </row>
     <row r="168" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B168" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C168" s="1">
         <v>3</v>
@@ -2394,7 +2395,7 @@
     </row>
     <row r="169" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B169" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C169" s="1">
         <v>2</v>
@@ -2402,7 +2403,7 @@
     </row>
     <row r="170" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B170" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C170" s="1">
         <v>4</v>
@@ -2410,7 +2411,7 @@
     </row>
     <row r="171" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B171" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C171" s="1">
         <v>2</v>
@@ -2418,7 +2419,7 @@
     </row>
     <row r="172" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B172" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C172" s="1">
         <v>5</v>
@@ -2426,7 +2427,7 @@
     </row>
     <row r="173" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B173" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C173" s="1">
         <v>5</v>
@@ -2434,7 +2435,7 @@
     </row>
     <row r="174" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B174" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C174" s="1">
         <v>6</v>
@@ -2442,7 +2443,7 @@
     </row>
     <row r="175" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B175" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C175" s="1">
         <v>7</v>
@@ -2450,7 +2451,7 @@
     </row>
     <row r="176" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B176" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C176" s="1">
         <v>9</v>
@@ -2458,7 +2459,7 @@
     </row>
     <row r="177" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B177" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C177" s="1">
         <v>8</v>
@@ -2466,7 +2467,7 @@
     </row>
     <row r="178" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B178" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C178" s="1">
         <v>10</v>
@@ -2474,7 +2475,7 @@
     </row>
     <row r="179" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B179" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C179" s="1">
         <v>8</v>
@@ -2482,7 +2483,7 @@
     </row>
     <row r="180" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B180" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C180" s="1">
         <v>10.5</v>
@@ -2490,7 +2491,7 @@
     </row>
     <row r="181" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B181" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C181" s="1">
         <v>10.5</v>
@@ -2498,7 +2499,7 @@
     </row>
     <row r="182" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B182" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C182" s="1">
         <v>10</v>
@@ -2506,7 +2507,7 @@
     </row>
     <row r="183" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B183" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C183" s="1">
         <v>10.5</v>
@@ -2514,7 +2515,7 @@
     </row>
     <row r="184" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B184" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C184" s="1">
         <v>10.5</v>
@@ -2522,10 +2523,10 @@
     </row>
     <row r="186" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A186" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B186" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="B186" s="1" t="s">
-        <v>178</v>
       </c>
       <c r="C186" s="1">
         <v>4</v>
@@ -2533,7 +2534,7 @@
     </row>
     <row r="187" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B187" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C187" s="1">
         <v>4</v>
@@ -2541,7 +2542,7 @@
     </row>
     <row r="188" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B188" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C188" s="1">
         <v>10</v>
@@ -2549,7 +2550,7 @@
     </row>
     <row r="189" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B189" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C189" s="1">
         <v>5</v>
@@ -2557,7 +2558,7 @@
     </row>
     <row r="190" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B190" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C190" s="1">
         <v>2</v>
@@ -2565,7 +2566,7 @@
     </row>
     <row r="191" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B191" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C191" s="1">
         <v>3</v>
@@ -2573,7 +2574,7 @@
     </row>
     <row r="192" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B192" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C192" s="1">
         <v>3</v>
@@ -2581,7 +2582,7 @@
     </row>
     <row r="193" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B193" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C193" s="1">
         <v>4</v>
@@ -2589,7 +2590,7 @@
     </row>
     <row r="194" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B194" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C194" s="1">
         <v>2</v>
@@ -2597,7 +2598,7 @@
     </row>
     <row r="195" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B195" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C195" s="1">
         <v>1</v>
@@ -2605,7 +2606,7 @@
     </row>
     <row r="196" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B196" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C196" s="1">
         <v>5</v>
@@ -2613,7 +2614,7 @@
     </row>
     <row r="197" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B197" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C197" s="1">
         <v>9</v>
@@ -2621,7 +2622,7 @@
     </row>
     <row r="198" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B198" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C198" s="1">
         <v>6</v>
@@ -2629,7 +2630,7 @@
     </row>
     <row r="199" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B199" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C199" s="1">
         <v>7</v>
@@ -2637,7 +2638,7 @@
     </row>
     <row r="200" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B200" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C200" s="1">
         <v>6</v>
@@ -2645,7 +2646,7 @@
     </row>
     <row r="201" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B201" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C201" s="1">
         <v>1</v>
@@ -2653,7 +2654,7 @@
     </row>
     <row r="202" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B202" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C202" s="1">
         <v>2</v>
@@ -2661,7 +2662,7 @@
     </row>
     <row r="203" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B203" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C203" s="1">
         <v>10.5</v>
@@ -2669,7 +2670,7 @@
     </row>
     <row r="204" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B204" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C204" s="1">
         <v>8</v>
@@ -2677,10 +2678,10 @@
     </row>
     <row r="206" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A206" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B206" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="B206" s="1" t="s">
-        <v>194</v>
       </c>
       <c r="C206" s="1">
         <v>3</v>
@@ -2688,7 +2689,7 @@
     </row>
     <row r="207" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B207" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C207" s="1">
         <v>3</v>
@@ -2704,7 +2705,7 @@
     </row>
     <row r="209" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B209" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C209" s="1">
         <v>6</v>
@@ -2712,7 +2713,7 @@
     </row>
     <row r="210" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B210" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C210" s="1">
         <v>7</v>
@@ -2720,7 +2721,7 @@
     </row>
     <row r="211" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B211" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C211" s="1">
         <v>1</v>
@@ -2728,7 +2729,7 @@
     </row>
     <row r="212" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B212" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C212" s="1">
         <v>1</v>
@@ -2736,7 +2737,7 @@
     </row>
     <row r="213" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B213" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C213" s="1">
         <v>4</v>
@@ -2744,7 +2745,7 @@
     </row>
     <row r="214" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B214" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C214" s="1">
         <v>5</v>
@@ -2752,7 +2753,7 @@
     </row>
     <row r="215" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B215" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C215" s="1">
         <v>2</v>
@@ -2760,7 +2761,7 @@
     </row>
     <row r="216" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B216" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C216" s="1">
         <v>4</v>
@@ -2768,7 +2769,7 @@
     </row>
     <row r="217" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B217" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C217" s="1">
         <v>2</v>
@@ -2776,7 +2777,7 @@
     </row>
     <row r="218" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B218" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C218" s="1">
         <v>5</v>
@@ -2784,7 +2785,7 @@
     </row>
     <row r="219" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B219" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C219" s="1">
         <v>8</v>
@@ -2792,7 +2793,7 @@
     </row>
     <row r="220" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B220" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C220" s="1">
         <v>7</v>
@@ -2800,7 +2801,7 @@
     </row>
     <row r="221" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B221" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C221" s="1">
         <v>6</v>
@@ -2808,7 +2809,7 @@
     </row>
     <row r="222" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B222" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C222" s="1">
         <v>7</v>
@@ -2816,7 +2817,7 @@
     </row>
     <row r="223" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B223" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C223" s="1">
         <v>9</v>
@@ -2828,10 +2829,10 @@
     </row>
     <row r="225" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A225" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B225" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="B225" s="1" t="s">
-        <v>211</v>
       </c>
       <c r="C225" s="1">
         <v>1</v>
@@ -2839,7 +2840,7 @@
     </row>
     <row r="226" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B226" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C226" s="1">
         <v>2</v>
@@ -2847,7 +2848,7 @@
     </row>
     <row r="227" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B227" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C227" s="1">
         <v>1</v>
@@ -2855,7 +2856,7 @@
     </row>
     <row r="228" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B228" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C228" s="1">
         <v>7</v>
@@ -2863,7 +2864,7 @@
     </row>
     <row r="229" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B229" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C229" s="1">
         <v>2</v>
@@ -2871,7 +2872,7 @@
     </row>
     <row r="230" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B230" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C230" s="1">
         <v>2</v>
@@ -2879,7 +2880,7 @@
     </row>
     <row r="231" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B231" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C231" s="1">
         <v>2</v>
@@ -2887,7 +2888,7 @@
     </row>
     <row r="232" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B232" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C232" s="1">
         <v>3</v>
@@ -2895,7 +2896,7 @@
     </row>
     <row r="233" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B233" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C233" s="1">
         <v>4</v>
@@ -2903,7 +2904,7 @@
     </row>
     <row r="234" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B234" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C234" s="1">
         <v>4</v>
@@ -2911,7 +2912,7 @@
     </row>
     <row r="235" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B235" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C235" s="1">
         <v>6</v>
@@ -2919,7 +2920,7 @@
     </row>
     <row r="236" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B236" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C236" s="1">
         <v>8</v>
@@ -2927,7 +2928,7 @@
     </row>
     <row r="237" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B237" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C237" s="1">
         <v>1</v>
@@ -2936,10 +2937,10 @@
     <row r="238" spans="1:3" ht="13" x14ac:dyDescent="0.15"/>
     <row r="239" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A239" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C239" s="1">
         <v>1</v>
@@ -2947,7 +2948,7 @@
     </row>
     <row r="240" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B240" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C240" s="1">
         <v>1</v>
@@ -2955,7 +2956,7 @@
     </row>
     <row r="241" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B241" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C241" s="1">
         <v>2</v>
@@ -2963,7 +2964,7 @@
     </row>
     <row r="242" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B242" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C242" s="1">
         <v>8</v>
@@ -2971,7 +2972,7 @@
     </row>
     <row r="243" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B243" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C243" s="1">
         <v>3</v>
@@ -2979,7 +2980,7 @@
     </row>
     <row r="244" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B244" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C244" s="1">
         <v>3</v>
@@ -2987,7 +2988,7 @@
     </row>
     <row r="245" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B245" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C245" s="1">
         <v>4</v>
@@ -2995,7 +2996,7 @@
     </row>
     <row r="246" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B246" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C246" s="1">
         <v>5</v>
@@ -3003,7 +3004,7 @@
     </row>
     <row r="247" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B247" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C247" s="1">
         <v>3</v>
@@ -3011,7 +3012,7 @@
     </row>
     <row r="248" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B248" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C248" s="1">
         <v>2</v>
@@ -3019,7 +3020,7 @@
     </row>
     <row r="249" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B249" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C249" s="1">
         <v>2</v>
@@ -3027,7 +3028,7 @@
     </row>
     <row r="250" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B250" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C250" s="1">
         <v>5</v>
@@ -3043,7 +3044,7 @@
     </row>
     <row r="252" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B252" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C252" s="1">
         <v>6</v>
@@ -3051,7 +3052,7 @@
     </row>
     <row r="253" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B253" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C253" s="1">
         <v>8</v>
@@ -3059,7 +3060,7 @@
     </row>
     <row r="254" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B254" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C254" s="1">
         <v>10.5</v>
@@ -3067,7 +3068,7 @@
     </row>
     <row r="255" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B255" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C255" s="1">
         <v>8</v>
@@ -3075,7 +3076,7 @@
     </row>
     <row r="256" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B256" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C256" s="1">
         <v>7</v>
@@ -3083,10 +3084,10 @@
     </row>
     <row r="258" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A258" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B258" s="1" t="s">
         <v>237</v>
-      </c>
-      <c r="B258" s="1" t="s">
-        <v>238</v>
       </c>
       <c r="C258" s="1">
         <v>3</v>
@@ -3094,7 +3095,7 @@
     </row>
     <row r="259" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B259" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C259" s="1">
         <v>9</v>
@@ -3102,7 +3103,7 @@
     </row>
     <row r="260" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B260" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C260" s="1">
         <v>4</v>
@@ -3110,7 +3111,7 @@
     </row>
     <row r="261" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B261" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C261" s="1">
         <v>6</v>
@@ -3118,7 +3119,7 @@
     </row>
     <row r="262" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B262" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C262" s="1">
         <v>5</v>
@@ -3126,7 +3127,7 @@
     </row>
     <row r="263" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B263" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C263" s="1">
         <v>5</v>
@@ -3134,7 +3135,7 @@
     </row>
     <row r="264" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B264" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C264" s="1">
         <v>9</v>
@@ -3150,7 +3151,7 @@
     </row>
     <row r="266" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B266" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C266" s="1">
         <v>10</v>
@@ -3158,7 +3159,7 @@
     </row>
     <row r="267" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B267" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C267" s="1">
         <v>7</v>
@@ -3166,7 +3167,7 @@
     </row>
     <row r="268" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B268" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C268" s="1">
         <v>8</v>
@@ -3174,7 +3175,7 @@
     </row>
     <row r="269" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B269" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C269" s="1">
         <v>2</v>
@@ -3182,7 +3183,7 @@
     </row>
     <row r="270" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B270" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C270" s="1">
         <v>4</v>
@@ -3190,7 +3191,7 @@
     </row>
     <row r="271" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B271" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C271" s="1">
         <v>1</v>

</xml_diff>